<commit_message>
Add Drone purchase on 장부
</commit_message>
<xml_diff>
--- a/AlwaysOn/장부.xlsx
+++ b/AlwaysOn/장부.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\MTDC\AlwaysOn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MTDC\AlwaysOn\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9588" windowHeight="1776"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9590" windowHeight="1780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>날짜</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -99,6 +99,18 @@
   </si>
   <si>
     <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지무근</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>드론 kit</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -197,7 +209,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -217,6 +229,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -279,7 +294,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -331,7 +346,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -536,20 +551,22 @@
   <dimension ref="B3:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E8" sqref="B8:E8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="3" width="8.59765625" style="1"/>
-    <col min="4" max="4" width="28.59765625" style="1" customWidth="1"/>
-    <col min="5" max="7" width="12.09765625" style="1" customWidth="1"/>
-    <col min="8" max="10" width="8.59765625" style="1"/>
+    <col min="1" max="1" width="8.58203125" style="1"/>
+    <col min="2" max="2" width="11.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.58203125" style="1"/>
+    <col min="4" max="4" width="28.58203125" style="1" customWidth="1"/>
+    <col min="5" max="7" width="12.08203125" style="1" customWidth="1"/>
+    <col min="8" max="10" width="8.58203125" style="1"/>
     <col min="11" max="11" width="18.5" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.59765625" style="1"/>
+    <col min="12" max="16384" width="8.58203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:11" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -572,7 +589,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:11" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -596,7 +613,7 @@
         <v>800000</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:11" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -620,10 +637,10 @@
       </c>
       <c r="K5" s="6">
         <f>K4-SUM(E4:E1048576)</f>
-        <v>630560</v>
+        <v>470130</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
@@ -640,7 +657,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
@@ -657,8 +674,22 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="E8" s="2"/>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B8" s="7">
+        <v>42893</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="2">
+        <v>160430</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Add 중간보고서, Change name of always-on docs
</commit_message>
<xml_diff>
--- a/AlwaysOn/장부.xlsx
+++ b/AlwaysOn/장부.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>날짜</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -122,11 +122,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>케이블</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아두이노 자이로 센서</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>충전 케이블</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -163,7 +183,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -223,13 +243,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -255,6 +299,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -571,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:K9"/>
+  <dimension ref="B3:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -639,8 +689,8 @@
       </c>
     </row>
     <row r="5" spans="2:11" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="1" t="s">
-        <v>1</v>
+      <c r="B5" s="7">
+        <v>42859</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>9</v>
@@ -658,14 +708,14 @@
         <v>18</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="K5" s="6">
-        <f>K4-SUM(E4:E1048576)</f>
-        <v>460130</v>
+        <f>SUM(E4:E1048576)</f>
+        <v>350070</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:11" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
@@ -684,10 +734,17 @@
       <c r="G6" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="J6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="10">
+        <f>K4-SUM(E4:E1048576)</f>
+        <v>449930</v>
+      </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B7" s="1" t="s">
-        <v>1</v>
+      <c r="B7" s="7">
+        <v>42876</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>16</v>
@@ -719,7 +776,7 @@
         <v>160430</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>20</v>
@@ -727,19 +784,42 @@
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E9" s="2">
         <v>10000</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B10" s="7">
+        <v>42923</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="2">
+        <v>10200</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>